<commit_message>
Made Radar a career part; moved Destination to InfoProps from PN; Anchor now also sets Destination.
Added Radar to Parts the TechTree.
</commit_message>
<xml_diff>
--- a/TechTree/data/Parts.xlsx
+++ b/TechTree/data/Parts.xlsx
@@ -20,7 +20,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="I18" authorId="0">
+    <comment ref="I19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="82">
   <si>
     <t>name</t>
   </si>
@@ -174,6 +174,18 @@
   </si>
   <si>
     <t>heavierRocketry</t>
+  </si>
+  <si>
+    <t>TCAModuleRadar</t>
+  </si>
+  <si>
+    <t>Radar Module</t>
+  </si>
+  <si>
+    <t>This module uses ship's radar (every ship has one, right?) to get the altitude above the surface and to avoide collisions with hills, mountains and buildings.</t>
+  </si>
+  <si>
+    <t>electrics</t>
   </si>
   <si>
     <t>TCAModuleHorizontalSpeedControl</t>
@@ -363,12 +375,19 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -402,11 +421,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -414,59 +433,59 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -555,10 +574,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y19"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -621,7 +640,7 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -641,7 +660,7 @@
         <v>22</v>
       </c>
       <c r="G2" s="4" t="n">
-        <f aca="false">$G$19*(F2+E2)</f>
+        <f aca="false">$G$20*(F2+E2)</f>
         <v>24650</v>
       </c>
       <c r="H2" s="4" t="n">
@@ -667,7 +686,7 @@
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -687,7 +706,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="4" t="n">
-        <f aca="false">$G$19*(F3+E3)</f>
+        <f aca="false">$G$20*(F3+E3)</f>
         <v>7650</v>
       </c>
       <c r="H3" s="4" t="n">
@@ -733,7 +752,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="6" t="n">
-        <f aca="false">$G$19*(F4+E4)</f>
+        <f aca="false">$G$20*(F4+E4)</f>
         <v>22100</v>
       </c>
       <c r="H4" s="6" t="n">
@@ -759,7 +778,7 @@
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
@@ -779,7 +798,7 @@
         <v>18</v>
       </c>
       <c r="G5" s="6" t="n">
-        <f aca="false">$G$19*(F5+E5)</f>
+        <f aca="false">$G$20*(F5+E5)</f>
         <v>20400</v>
       </c>
       <c r="H5" s="6" t="n">
@@ -825,7 +844,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="8" t="n">
-        <f aca="false">$G$19*(F6+E6)</f>
+        <f aca="false">$G$20*(F6+E6)</f>
         <v>17000</v>
       </c>
       <c r="H6" s="8" t="n">
@@ -871,7 +890,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="8" t="n">
-        <f aca="false">$G$19*(F7+E7)</f>
+        <f aca="false">$G$20*(F7+E7)</f>
         <v>7650</v>
       </c>
       <c r="H7" s="8" t="n">
@@ -917,7 +936,7 @@
         <v>8</v>
       </c>
       <c r="G8" s="8" t="n">
-        <f aca="false">$G$19*(F8+E8)</f>
+        <f aca="false">$G$20*(F8+E8)</f>
         <v>11050</v>
       </c>
       <c r="H8" s="8" t="n">
@@ -963,7 +982,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="8" t="n">
-        <f aca="false">$G$19*(F9+E9)</f>
+        <f aca="false">$G$20*(F9+E9)</f>
         <v>10200</v>
       </c>
       <c r="H9" s="8" t="n">
@@ -1009,7 +1028,7 @@
         <v>12</v>
       </c>
       <c r="G10" s="8" t="n">
-        <f aca="false">$G$19*(F10+E10)</f>
+        <f aca="false">$G$20*(F10+E10)</f>
         <v>14450</v>
       </c>
       <c r="H10" s="8" t="n">
@@ -1035,7 +1054,7 @@
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
         <v>45</v>
       </c>
@@ -1052,15 +1071,13 @@
         <v>4</v>
       </c>
       <c r="F11" s="10" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G11" s="10" t="n">
-        <f aca="false">$G$19*(F11+E11)</f>
-        <v>16150</v>
-      </c>
-      <c r="H11" s="10" t="n">
-        <v>5560</v>
-      </c>
+        <f aca="false">$G$20*(F11+E11)</f>
+        <v>18700</v>
+      </c>
+      <c r="H11" s="10"/>
       <c r="I11" s="10" t="s">
         <v>13</v>
       </c>
@@ -1081,7 +1098,7 @@
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
         <v>49</v>
       </c>
@@ -1098,14 +1115,14 @@
         <v>4</v>
       </c>
       <c r="F12" s="10" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G12" s="10" t="n">
-        <f aca="false">$G$19*(F12+E12)</f>
-        <v>6800</v>
+        <f aca="false">$G$20*(F12+E12)</f>
+        <v>16150</v>
       </c>
       <c r="H12" s="10" t="n">
-        <v>3280</v>
+        <v>5560</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>13</v>
@@ -1127,8 +1144,8 @@
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
+    <row r="13" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
         <v>53</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -1144,14 +1161,14 @@
         <v>4</v>
       </c>
       <c r="F13" s="10" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G13" s="10" t="n">
-        <f aca="false">$G$19*(F13+E13)</f>
-        <v>10200</v>
+        <f aca="false">$G$20*(F13+E13)</f>
+        <v>6800</v>
       </c>
       <c r="H13" s="10" t="n">
-        <v>5183.3</v>
+        <v>3280</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>13</v>
@@ -1173,8 +1190,8 @@
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
     </row>
-    <row r="14" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
+    <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -1190,14 +1207,14 @@
         <v>4</v>
       </c>
       <c r="F14" s="10" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G14" s="10" t="n">
-        <f aca="false">$G$19*(F14+E14)</f>
-        <v>11900</v>
+        <f aca="false">$G$20*(F14+E14)</f>
+        <v>10200</v>
       </c>
       <c r="H14" s="10" t="n">
-        <v>8733.3</v>
+        <v>5183.3</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>13</v>
@@ -1220,32 +1237,32 @@
       <c r="Y14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="13" t="n">
-        <v>3</v>
-      </c>
-      <c r="F15" s="13" t="n">
-        <v>12</v>
-      </c>
-      <c r="G15" s="13" t="n">
-        <f aca="false">$G$19*(F15+E15)</f>
-        <v>12750</v>
-      </c>
-      <c r="H15" s="13" t="n">
-        <v>3200</v>
-      </c>
-      <c r="I15" s="13" t="s">
+      <c r="E15" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F15" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="G15" s="10" t="n">
+        <f aca="false">$G$20*(F15+E15)</f>
+        <v>11900</v>
+      </c>
+      <c r="H15" s="10" t="n">
+        <v>8733.3</v>
+      </c>
+      <c r="I15" s="10" t="s">
         <v>13</v>
       </c>
       <c r="J15" s="3"/>
@@ -1282,14 +1299,14 @@
         <v>3</v>
       </c>
       <c r="F16" s="13" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G16" s="13" t="n">
-        <f aca="false">$G$19*(F16+E16)</f>
-        <v>7650</v>
+        <f aca="false">$G$20*(F16+E16)</f>
+        <v>12750</v>
       </c>
       <c r="H16" s="13" t="n">
-        <v>3128.6</v>
+        <v>3200</v>
       </c>
       <c r="I16" s="13" t="s">
         <v>13</v>
@@ -1311,7 +1328,7 @@
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
     </row>
-    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
         <v>69</v>
       </c>
@@ -1328,14 +1345,14 @@
         <v>3</v>
       </c>
       <c r="F17" s="13" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G17" s="13" t="n">
-        <f aca="false">$G$19*(F17+E17)</f>
-        <v>5950</v>
+        <f aca="false">$G$20*(F17+E17)</f>
+        <v>7650</v>
       </c>
       <c r="H17" s="13" t="n">
-        <v>2233.3</v>
+        <v>3128.6</v>
       </c>
       <c r="I17" s="13" t="s">
         <v>13</v>
@@ -1357,33 +1374,33 @@
       <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
     </row>
-    <row r="18" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="s">
+    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="16" t="n">
-        <v>2</v>
-      </c>
-      <c r="F18" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="G18" s="16" t="n">
-        <f aca="false">$G$19*(F18+E18)</f>
-        <v>10200</v>
-      </c>
-      <c r="H18" s="16" t="n">
-        <v>1566.7</v>
-      </c>
-      <c r="I18" s="16" t="s">
+      <c r="E18" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="F18" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="G18" s="13" t="n">
+        <f aca="false">$G$20*(F18+E18)</f>
+        <v>5950</v>
+      </c>
+      <c r="H18" s="13" t="n">
+        <v>2233.3</v>
+      </c>
+      <c r="I18" s="13" t="s">
         <v>13</v>
       </c>
       <c r="J18" s="3"/>
@@ -1403,20 +1420,35 @@
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="19" t="s">
+    <row r="19" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="19" t="n">
-        <v>850</v>
-      </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="B19" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="G19" s="16" t="n">
+        <f aca="false">$G$20*(F19+E19)</f>
+        <v>10200</v>
+      </c>
+      <c r="H19" s="16" t="n">
+        <v>1566.7</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -1434,6 +1466,37 @@
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
     </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="19" t="n">
+        <v>850</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Moved Executors to Components subfolder. Added ToOrbitAutopilot to TechTree.
</commit_message>
<xml_diff>
--- a/TechTree/data/Parts.xlsx
+++ b/TechTree/data/Parts.xlsx
@@ -16,7 +16,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="I23">
+    <comment authorId="0" ref="I24">
       <text>
         <t xml:space="preserve">Squad/Parts/Command/probeCoreOcto2/model</t>
       </text>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="98">
   <si>
     <t>name</t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>heavierRocketry</t>
+  </si>
+  <si>
+    <t>TCAModuleToOrbitAutopilot</t>
+  </si>
+  <si>
+    <t>To Orbit Autopilot</t>
+  </si>
+  <si>
+    <t>This autopilot launches a vessel into circular orbit with given radius and inclination using double-maneuver technique. Both ascending/descending and prograde/retrograde orbits are supported.</t>
   </si>
   <si>
     <t>TCAModuleRadar</t>
@@ -612,7 +621,7 @@
         <v>22.0</v>
       </c>
       <c r="G2" s="8" t="str">
-        <f t="shared" ref="G2:G23" si="1">$G$24*(F2+E2)</f>
+        <f t="shared" ref="G2:G24" si="1">$G$25*(F2+E2)</f>
         <v>24650</v>
       </c>
       <c r="H2" s="8">
@@ -1184,31 +1193,33 @@
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
     </row>
-    <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="20" t="s">
+    <row r="15" ht="23.25" customHeight="1">
+      <c r="A15" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="20" t="s">
-        <v>61</v>
+      <c r="D15" s="15" t="s">
+        <v>57</v>
       </c>
-      <c r="E15" s="20">
-        <v>4.0</v>
+      <c r="E15" s="18">
+        <v>5.0</v>
       </c>
-      <c r="F15" s="20">
-        <v>18.0</v>
+      <c r="F15" s="18">
+        <v>15.0</v>
       </c>
-      <c r="G15" s="20" t="str">
+      <c r="G15" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>18700</v>
+        <v>17000</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20" t="s">
+      <c r="H15" s="18">
+        <v>51500.0</v>
+      </c>
+      <c r="I15" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J15" s="5"/>
@@ -1229,31 +1240,29 @@
       <c r="Y15" s="5"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="C16" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="D16" s="20" t="s">
         <v>64</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>65</v>
       </c>
       <c r="E16" s="20">
         <v>4.0</v>
       </c>
       <c r="F16" s="20">
-        <v>15.0</v>
+        <v>18.0</v>
       </c>
       <c r="G16" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>16150</v>
+        <v>18700</v>
       </c>
-      <c r="H16" s="20">
-        <v>5560.0</v>
-      </c>
+      <c r="H16" s="20"/>
       <c r="I16" s="20" t="s">
         <v>13</v>
       </c>
@@ -1274,31 +1283,31 @@
       <c r="X16" s="5"/>
       <c r="Y16" s="5"/>
     </row>
-    <row r="17" ht="23.25" customHeight="1">
+    <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="C17" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="D17" s="22" t="s">
         <v>68</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>69</v>
       </c>
       <c r="E17" s="20">
         <v>4.0</v>
       </c>
       <c r="F17" s="20">
-        <v>4.0</v>
+        <v>15.0</v>
       </c>
       <c r="G17" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>6800</v>
+        <v>16150</v>
       </c>
       <c r="H17" s="20">
-        <v>3280.0</v>
+        <v>5560.0</v>
       </c>
       <c r="I17" s="20" t="s">
         <v>13</v>
@@ -1320,31 +1329,31 @@
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
     </row>
-    <row r="18" ht="18.75" customHeight="1">
-      <c r="A18" s="24" t="s">
+    <row r="18" ht="23.25" customHeight="1">
+      <c r="A18" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="C18" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="D18" s="22" t="s">
         <v>72</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>73</v>
       </c>
       <c r="E18" s="20">
         <v>4.0</v>
       </c>
       <c r="F18" s="20">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
       <c r="G18" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>10200</v>
+        <v>6800</v>
       </c>
       <c r="H18" s="20">
-        <v>5183.3</v>
+        <v>3280.0</v>
       </c>
       <c r="I18" s="20" t="s">
         <v>13</v>
@@ -1366,31 +1375,31 @@
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
     </row>
-    <row r="19" ht="23.25" customHeight="1">
-      <c r="A19" s="22" t="s">
+    <row r="19" ht="18.75" customHeight="1">
+      <c r="A19" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="C19" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="D19" s="22" t="s">
         <v>76</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>77</v>
       </c>
       <c r="E19" s="20">
         <v>4.0</v>
       </c>
       <c r="F19" s="20">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="G19" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>11900</v>
+        <v>10200</v>
       </c>
       <c r="H19" s="20">
-        <v>8733.3</v>
+        <v>5183.3</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>13</v>
@@ -1413,32 +1422,32 @@
       <c r="Y19" s="5"/>
     </row>
     <row r="20" ht="23.25" customHeight="1">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="C20" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="D20" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="25" t="s">
-        <v>81</v>
+      <c r="E20" s="20">
+        <v>4.0</v>
       </c>
-      <c r="E20" s="27">
-        <v>3.0</v>
+      <c r="F20" s="20">
+        <v>10.0</v>
       </c>
-      <c r="F20" s="27">
-        <v>12.0</v>
+      <c r="G20" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>11900</v>
       </c>
-      <c r="G20" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>12750</v>
+      <c r="H20" s="20">
+        <v>8733.3</v>
       </c>
-      <c r="H20" s="27">
-        <v>3200.0</v>
-      </c>
-      <c r="I20" s="27" t="s">
+      <c r="I20" s="20" t="s">
         <v>13</v>
       </c>
       <c r="J20" s="5"/>
@@ -1460,29 +1469,29 @@
     </row>
     <row r="21" ht="23.25" customHeight="1">
       <c r="A21" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="C21" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="D21" s="25" t="s">
         <v>84</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>85</v>
       </c>
       <c r="E21" s="27">
         <v>3.0</v>
       </c>
       <c r="F21" s="27">
-        <v>6.0</v>
+        <v>12.0</v>
       </c>
       <c r="G21" s="27" t="str">
         <f t="shared" si="1"/>
-        <v>7650</v>
+        <v>12750</v>
       </c>
       <c r="H21" s="27">
-        <v>3128.6</v>
+        <v>3200.0</v>
       </c>
       <c r="I21" s="27" t="s">
         <v>13</v>
@@ -1506,29 +1515,29 @@
     </row>
     <row r="22" ht="23.25" customHeight="1">
       <c r="A22" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="C22" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="D22" s="25" t="s">
         <v>88</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>89</v>
       </c>
       <c r="E22" s="27">
         <v>3.0</v>
       </c>
       <c r="F22" s="27">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="G22" s="27" t="str">
         <f t="shared" si="1"/>
-        <v>5950</v>
+        <v>7650</v>
       </c>
       <c r="H22" s="27">
-        <v>2233.3</v>
+        <v>3128.6</v>
       </c>
       <c r="I22" s="27" t="s">
         <v>13</v>
@@ -1551,32 +1560,32 @@
       <c r="Y22" s="5"/>
     </row>
     <row r="23" ht="23.25" customHeight="1">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="C23" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="D23" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="29" t="s">
-        <v>93</v>
+      <c r="E23" s="27">
+        <v>3.0</v>
       </c>
-      <c r="E23" s="32">
-        <v>2.0</v>
+      <c r="F23" s="27">
+        <v>4.0</v>
       </c>
-      <c r="F23" s="32">
-        <v>10.0</v>
+      <c r="G23" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v>5950</v>
       </c>
-      <c r="G23" s="32" t="str">
-        <f t="shared" si="1"/>
-        <v>10200</v>
+      <c r="H23" s="27">
+        <v>2233.3</v>
       </c>
-      <c r="H23" s="32">
-        <v>1566.7</v>
-      </c>
-      <c r="I23" s="32" t="s">
+      <c r="I23" s="27" t="s">
         <v>13</v>
       </c>
       <c r="J23" s="5"/>
@@ -1596,20 +1605,35 @@
       <c r="X23" s="5"/>
       <c r="Y23" s="5"/>
     </row>
-    <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="34" t="s">
+    <row r="24" ht="23.25" customHeight="1">
+      <c r="A24" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="G24" s="34">
-        <v>850.0</v>
+      <c r="C24" s="31" t="s">
+        <v>95</v>
       </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+      <c r="D24" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="32">
+        <v>2.0</v>
+      </c>
+      <c r="F24" s="32">
+        <v>10.0</v>
+      </c>
+      <c r="G24" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v>10200</v>
+      </c>
+      <c r="H24" s="32">
+        <v>1566.7</v>
+      </c>
+      <c r="I24" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -1633,8 +1657,12 @@
       <c r="C25" s="33"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25" s="34">
+        <v>850.0</v>
+      </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
@@ -28114,6 +28142,33 @@
       <c r="X1005" s="5"/>
       <c r="Y1005" s="5"/>
     </row>
+    <row r="1006" ht="12.75" customHeight="1">
+      <c r="A1006" s="5"/>
+      <c r="B1006" s="5"/>
+      <c r="C1006" s="33"/>
+      <c r="D1006" s="5"/>
+      <c r="E1006" s="5"/>
+      <c r="F1006" s="5"/>
+      <c r="G1006" s="5"/>
+      <c r="H1006" s="5"/>
+      <c r="I1006" s="5"/>
+      <c r="J1006" s="5"/>
+      <c r="K1006" s="5"/>
+      <c r="L1006" s="5"/>
+      <c r="M1006" s="5"/>
+      <c r="N1006" s="5"/>
+      <c r="O1006" s="5"/>
+      <c r="P1006" s="5"/>
+      <c r="Q1006" s="5"/>
+      <c r="R1006" s="5"/>
+      <c r="S1006" s="5"/>
+      <c r="T1006" s="5"/>
+      <c r="U1006" s="5"/>
+      <c r="V1006" s="5"/>
+      <c r="W1006" s="5"/>
+      <c r="X1006" s="5"/>
+      <c r="Y1006" s="5"/>
+    </row>
   </sheetData>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>